<commit_message>
Added Clasification by svm and ClaTree
</commit_message>
<xml_diff>
--- a/logistic/DATOS.xlsx
+++ b/logistic/DATOS.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unaledu-my.sharepoint.com/personal/clochoac_unal_edu_co/Documents/Inteligencia artificial/Proyecto/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cesar\Documents\GitHub\Proyecto-IA\logistic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="2E0D20F72FE39269ED8F365351D3DF71D6D4EDC3" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{BF0555C6-327A-4A2E-867D-BBBCD3420B7F}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Direcciones" sheetId="2" r:id="rId2"/>
+    <sheet name="dev" sheetId="3" r:id="rId2"/>
+    <sheet name="rep" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$K$94</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="112">
   <si>
     <t>REGIONAL</t>
   </si>
@@ -282,6 +282,84 @@
   </si>
   <si>
     <t>NO</t>
+  </si>
+  <si>
+    <t>F. PROGRAMADA DE ENTREGA</t>
+  </si>
+  <si>
+    <t>Supertiendas y Droguerias Olimpicas S.A.</t>
+  </si>
+  <si>
+    <t>Almacenes Exito S.A</t>
+  </si>
+  <si>
+    <t>Centro de Distribución Caribe Parque Industrial Malambo PIMSA</t>
+  </si>
+  <si>
+    <t>Makro Supermayorista S.A.S.</t>
+  </si>
+  <si>
+    <t>JERONIMO MARTINS</t>
+  </si>
+  <si>
+    <t>VIA LA CORDIALIDAD KM 3 VILLA GALAPA</t>
+  </si>
+  <si>
+    <t>PriceSmart Colombia S.A.S</t>
+  </si>
+  <si>
+    <t>ESTADO CONTABLE</t>
+  </si>
+  <si>
+    <t>DEV</t>
+  </si>
+  <si>
+    <t>NO RECIBIDA</t>
+  </si>
+  <si>
+    <t>DEV- 41445</t>
+  </si>
+  <si>
+    <t>Supertiendas y Droguerias Olimpica S.A.</t>
+  </si>
+  <si>
+    <t>DEV-41444</t>
+  </si>
+  <si>
+    <t>INVERCOMER DEL CARIBE</t>
+  </si>
+  <si>
+    <t>DEV-41448</t>
+  </si>
+  <si>
+    <t>DEV-41492</t>
+  </si>
+  <si>
+    <t>DEV-41400</t>
+  </si>
+  <si>
+    <t>DEV-41398</t>
+  </si>
+  <si>
+    <t>DEV-41399</t>
+  </si>
+  <si>
+    <t>CONTABILIDAD</t>
+  </si>
+  <si>
+    <t>DEV- 41489</t>
+  </si>
+  <si>
+    <t>DEV-41490</t>
+  </si>
+  <si>
+    <t>DEV-41446</t>
+  </si>
+  <si>
+    <t>DEV-41432</t>
+  </si>
+  <si>
+    <t>DEV-41491</t>
   </si>
 </sst>
 </file>
@@ -895,7 +973,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1012,6 +1090,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1151,10 +1240,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="141414"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="F8F8F8"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1411,8 +1500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L401"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L42" sqref="A42:L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -5903,19 +5992,731 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82D101F1-01BD-4C76-903E-CFDCB5D575A7}">
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="6" width="11.42578125" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>15481</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="44" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>15491</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>15492</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
+        <v>15508</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1">
+        <v>15509</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1">
+        <v>15518</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1">
+        <v>15519</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1">
+        <v>15521</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1">
+        <v>15523</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1">
+        <v>15527</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1">
+        <v>15540</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1">
+        <v>15542</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:L17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="4" width="11.42578125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="1"/>
+    <col min="5" max="11" width="11.42578125" style="1"/>
+    <col min="12" max="12" width="40.7109375" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="11.42578125" style="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="2:12" ht="60">
+      <c r="B1" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="41" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="33" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="2:12">
+      <c r="B2" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="36">
+        <v>15645</v>
+      </c>
+      <c r="D2" s="45">
+        <v>181896</v>
+      </c>
+      <c r="E2" s="37">
+        <v>43008</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="L2" s="36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12">
+      <c r="B3" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" s="36">
+        <v>15647</v>
+      </c>
+      <c r="D3" s="45">
+        <v>363792</v>
+      </c>
+      <c r="E3" s="37">
+        <v>43011</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="L3" s="36" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12">
+      <c r="B4" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="36">
+        <v>15648</v>
+      </c>
+      <c r="D4" s="45">
+        <v>2566944</v>
+      </c>
+      <c r="E4" s="37">
+        <v>43012</v>
+      </c>
+      <c r="F4" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="L4" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12">
+      <c r="B5" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="36">
+        <v>15649</v>
+      </c>
+      <c r="D5" s="45">
+        <v>227808</v>
+      </c>
+      <c r="E5" s="37">
+        <v>43012</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="L5" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12">
+      <c r="B6" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="36">
+        <v>15650</v>
+      </c>
+      <c r="D6" s="45">
+        <v>356400</v>
+      </c>
+      <c r="E6" s="37">
+        <v>43012</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="L6" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12">
+      <c r="B7" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="36">
+        <v>15653</v>
+      </c>
+      <c r="D7" s="45">
+        <v>261312</v>
+      </c>
+      <c r="E7" s="37">
+        <v>43006</v>
+      </c>
+      <c r="F7" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
+      <c r="J7" s="42"/>
+      <c r="K7" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="L7" s="36" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12">
+      <c r="B8" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="36">
+        <v>15654</v>
+      </c>
+      <c r="D8" s="45">
+        <v>790920</v>
+      </c>
+      <c r="E8" s="37">
+        <v>43012</v>
+      </c>
+      <c r="F8" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="L8" s="36" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12">
+      <c r="B9" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="36">
+        <v>15655</v>
+      </c>
+      <c r="D9" s="45">
+        <v>1067328</v>
+      </c>
+      <c r="E9" s="37">
+        <v>43012</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="L9" s="36" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12">
+      <c r="B10" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="36">
+        <v>15656</v>
+      </c>
+      <c r="D10" s="45">
+        <v>2741400</v>
+      </c>
+      <c r="E10" s="37">
+        <v>43012</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="L10" s="36" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12">
+      <c r="B11" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" s="43">
+        <v>15657</v>
+      </c>
+      <c r="D11" s="45">
+        <v>657072</v>
+      </c>
+      <c r="E11" s="37">
+        <v>43012</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="L11" s="36" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12">
+      <c r="B12" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" s="43">
+        <v>15658</v>
+      </c>
+      <c r="D12" s="45">
+        <v>296352</v>
+      </c>
+      <c r="E12" s="37">
+        <v>43012</v>
+      </c>
+      <c r="F12" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="L12" s="36" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12">
+      <c r="B13" s="36" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" s="36">
+        <v>15659</v>
+      </c>
+      <c r="D13" s="45">
+        <v>6126120</v>
+      </c>
+      <c r="E13" s="37">
+        <v>43012</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="42"/>
+      <c r="K13" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="L13" s="36" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12">
+      <c r="B14" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" s="36">
+        <v>15660</v>
+      </c>
+      <c r="D14" s="45">
+        <v>5973000</v>
+      </c>
+      <c r="E14" s="37">
+        <v>43012</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="42"/>
+      <c r="K14" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="L14" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12">
+      <c r="B15" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="43">
+        <v>15661</v>
+      </c>
+      <c r="D15" s="45">
+        <v>74088</v>
+      </c>
+      <c r="E15" s="37">
+        <v>43012</v>
+      </c>
+      <c r="F15" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" s="42"/>
+      <c r="I15" s="42"/>
+      <c r="J15" s="42"/>
+      <c r="K15" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="L15" s="36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12">
+      <c r="B16" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="36">
+        <v>15662</v>
+      </c>
+      <c r="D16" s="45">
+        <v>5970780</v>
+      </c>
+      <c r="E16" s="37">
+        <v>43012</v>
+      </c>
+      <c r="F16" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
+      <c r="K16" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="L16" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="30">
+      <c r="A17" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="9">
+        <v>15488</v>
+      </c>
+      <c r="D17" s="8">
+        <v>12096900</v>
+      </c>
+      <c r="E17" s="10">
+        <v>42962</v>
+      </c>
+      <c r="F17" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="I17" s="28">
+        <v>0.4375</v>
+      </c>
+      <c r="J17" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="K17" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="L17" s="36" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Get From Database Dispatches
Added Get From Database Dispatches, Fixed Minor Bugs
</commit_message>
<xml_diff>
--- a/logistic/DATOS.xlsx
+++ b/logistic/DATOS.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cesar\Documents\GitHub\Proyecto-IA\logistic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cesar\OneDrive - Universidad Nacional de Colombia\Inteligencia artificial\Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="38" documentId="61BD013F700551E89C5D0505C8FC255AD66F6F1A" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{E95DA4C3-5D05-4F50-B52B-5A9D70B94DF7}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -293,9 +294,6 @@
     <t>Almacenes Exito S.A</t>
   </si>
   <si>
-    <t>Centro de Distribución Caribe Parque Industrial Malambo PIMSA</t>
-  </si>
-  <si>
     <t>Makro Supermayorista S.A.S.</t>
   </si>
   <si>
@@ -360,6 +358,9 @@
   </si>
   <si>
     <t>DEV-41491</t>
+  </si>
+  <si>
+    <t>Parque Industrial Malambo PIMSAParque Industrial Malambo PIMSA</t>
   </si>
 </sst>
 </file>
@@ -1156,6 +1157,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1172,10 +1241,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="141414"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="F8F8F8"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1432,8 +1501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L401"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L42" sqref="A42:L42"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -5942,10 +6011,10 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
@@ -5956,13 +6025,13 @@
         <v>15481</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="44" t="s">
         <v>97</v>
-      </c>
-      <c r="D2" s="44" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -5970,13 +6039,13 @@
         <v>15491</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -5984,13 +6053,13 @@
         <v>15492</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -5998,13 +6067,13 @@
         <v>15508</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -6012,13 +6081,13 @@
         <v>15509</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -6026,13 +6095,13 @@
         <v>15518</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -6040,13 +6109,13 @@
         <v>15519</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -6054,10 +6123,10 @@
         <v>15521</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>88</v>
@@ -6068,13 +6137,13 @@
         <v>15523</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -6082,13 +6151,13 @@
         <v>15527</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -6096,10 +6165,10 @@
         <v>15540</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>88</v>
@@ -6110,13 +6179,13 @@
         <v>15542</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -6126,17 +6195,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L17"/>
+  <dimension ref="B1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L17" sqref="A17:L17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="4" width="11.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" style="1" customWidth="1"/>
+    <col min="3" max="4" width="11.42578125" style="1" customWidth="1"/>
     <col min="5" max="11" width="11.42578125" style="1"/>
-    <col min="12" max="12" width="40.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="30.28515625" style="1" customWidth="1"/>
     <col min="13" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
@@ -6259,7 +6330,7 @@
         <v>85</v>
       </c>
       <c r="L4" s="36" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="2:12">
@@ -6288,7 +6359,7 @@
         <v>85</v>
       </c>
       <c r="L5" s="36" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="2:12">
@@ -6317,12 +6388,12 @@
         <v>85</v>
       </c>
       <c r="L6" s="36" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="2:12">
       <c r="B7" s="36" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C7" s="36">
         <v>15653</v>
@@ -6351,7 +6422,7 @@
     </row>
     <row r="8" spans="2:12">
       <c r="B8" s="36" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C8" s="36">
         <v>15654</v>
@@ -6380,7 +6451,7 @@
     </row>
     <row r="9" spans="2:12">
       <c r="B9" s="36" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C9" s="36">
         <v>15655</v>
@@ -6409,7 +6480,7 @@
     </row>
     <row r="10" spans="2:12">
       <c r="B10" s="36" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C10" s="36">
         <v>15656</v>
@@ -6438,7 +6509,7 @@
     </row>
     <row r="11" spans="2:12">
       <c r="B11" s="36" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C11" s="43">
         <v>15657</v>
@@ -6462,12 +6533,12 @@
         <v>85</v>
       </c>
       <c r="L11" s="36" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="2:12">
       <c r="B12" s="36" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C12" s="43">
         <v>15658</v>
@@ -6491,12 +6562,12 @@
         <v>85</v>
       </c>
       <c r="L12" s="36" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="2:12">
       <c r="B13" s="36" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C13" s="36">
         <v>15659</v>
@@ -6549,7 +6620,7 @@
         <v>85</v>
       </c>
       <c r="L14" s="36" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="2:12">
@@ -6607,22 +6678,12 @@
         <v>85</v>
       </c>
       <c r="L16" s="36" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="10"/>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="6:7">
       <c r="F17" s="24"/>
       <c r="G17" s="12"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>